<commit_message>
add idea mysql note
</commit_message>
<xml_diff>
--- a/成考资料/22级河北工程大学考试名单.xlsx
+++ b/成考资料/22级河北工程大学考试名单.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28125" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>7</t>
     </r>
@@ -98,7 +98,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>9</t>
     </r>
@@ -114,7 +114,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>8:30</t>
     </r>
@@ -130,7 +130,7 @@
       <rPr>
         <sz val="12"/>
         <rFont val="Times New Roman"/>
-        <charset val="134"/>
+        <family val="1"/>
       </rPr>
       <t>10:00</t>
     </r>
@@ -388,15 +388,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,143 +432,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -585,10 +444,16 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,192 +462,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -790,270 +475,28 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="58">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1078,22 +521,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1102,71 +545,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="58">
+  <cellStyles count="10">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="常规 3 10" xfId="9"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="10" builtinId="40"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8"/>
-    <cellStyle name="百分比" xfId="12" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="13" builtinId="9"/>
-    <cellStyle name="注释" xfId="14" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="15" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="16" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="17" builtinId="11"/>
-    <cellStyle name="常规 5 2" xfId="18"/>
-    <cellStyle name="标题" xfId="19" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="20" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="21" builtinId="16"/>
-    <cellStyle name="常规 9" xfId="22"/>
-    <cellStyle name="标题 2" xfId="23" builtinId="17"/>
-    <cellStyle name="常规 4 11" xfId="24"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="25" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="26" builtinId="18"/>
-    <cellStyle name="常规 6 7" xfId="27"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="28" builtinId="44"/>
-    <cellStyle name="输出" xfId="29" builtinId="21"/>
-    <cellStyle name="计算" xfId="30" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="31" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="32" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="33" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="34" builtinId="24"/>
-    <cellStyle name="汇总" xfId="35" builtinId="25"/>
-    <cellStyle name="好" xfId="36" builtinId="26"/>
-    <cellStyle name="适中" xfId="37" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="38" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="39" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="40" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="41" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="42" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="43" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="44" builtinId="37"/>
-    <cellStyle name="常规 3 2" xfId="45"/>
-    <cellStyle name="强调文字颜色 4" xfId="46" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="47" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="48" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="49" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="50" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="51" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="52" builtinId="49"/>
-    <cellStyle name="常规 10" xfId="53"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="54" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="55" builtinId="52"/>
-    <cellStyle name="常规 2" xfId="56"/>
-    <cellStyle name="常规 7 7" xfId="57"/>
+    <cellStyle name="常规 10" xfId="7"/>
+    <cellStyle name="常规 2" xfId="8"/>
+    <cellStyle name="常规 3 10" xfId="1"/>
+    <cellStyle name="常规 3 2" xfId="6"/>
+    <cellStyle name="常规 4 11" xfId="4"/>
+    <cellStyle name="常规 5 2" xfId="2"/>
+    <cellStyle name="常规 6 7" xfId="5"/>
+    <cellStyle name="常规 7 7" xfId="9"/>
+    <cellStyle name="常规 9" xfId="3"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="00FF0000"/>
+      <color rgb="FFFF0000"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1458,40 +878,39 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="11.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1666666666667" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.125" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.35" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.38333333333333" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.275" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6.375" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.25" style="1" customWidth="1"/>
     <col min="10" max="10" width="31.875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.8916666666667" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.875" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" style="1" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5166666666667" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6583333333333" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11.625" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="14.25" spans="1:14">
+    <row r="1" spans="1:14" ht="14.25" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1535,7 +954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1575,7 +994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
@@ -1615,7 +1034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>26</v>
       </c>
@@ -1655,7 +1074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -1695,7 +1114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -1735,7 +1154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -1775,7 +1194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -1815,7 +1234,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>36</v>
       </c>
@@ -1855,7 +1274,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>38</v>
       </c>
@@ -1895,7 +1314,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>40</v>
       </c>
@@ -1935,7 +1354,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
@@ -1975,7 +1394,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>44</v>
       </c>
@@ -2015,7 +1434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
@@ -2055,7 +1474,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
         <v>48</v>
       </c>
@@ -2095,7 +1514,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
         <v>50</v>
       </c>
@@ -2135,47 +1554,47 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" s="1" customFormat="1" ht="15.75" spans="1:14">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:14" s="23" customFormat="1" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A17" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="10" t="s">
+      <c r="E17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="11"/>
-      <c r="I17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="10" t="s">
+      <c r="H17" s="19"/>
+      <c r="I17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="L17" s="10"/>
-      <c r="M17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N17" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" s="1" customFormat="1" ht="15.75" spans="1:14">
+      <c r="L17" s="18"/>
+      <c r="M17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>57</v>
       </c>
@@ -2215,7 +1634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>59</v>
       </c>
@@ -2255,7 +1674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
         <v>61</v>
       </c>
@@ -2295,7 +1714,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
         <v>63</v>
       </c>
@@ -2335,7 +1754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="22" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
         <v>66</v>
       </c>
@@ -2375,7 +1794,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
         <v>68</v>
       </c>
@@ -2415,7 +1834,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="24" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
         <v>70</v>
       </c>
@@ -2455,7 +1874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="25" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A25" s="3" t="s">
         <v>72</v>
       </c>
@@ -2495,7 +1914,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="26" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
@@ -2535,7 +1954,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="27" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>78</v>
       </c>
@@ -2575,7 +1994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>81</v>
       </c>
@@ -2615,7 +2034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="29" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>83</v>
       </c>
@@ -2655,7 +2074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="30" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A30" s="14" t="s">
         <v>85</v>
       </c>
@@ -2695,7 +2114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="31" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>87</v>
       </c>
@@ -2735,7 +2154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="32" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>90</v>
       </c>
@@ -2775,7 +2194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>92</v>
       </c>
@@ -2815,7 +2234,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>94</v>
       </c>
@@ -2855,7 +2274,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="35" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>96</v>
       </c>
@@ -2895,7 +2314,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" s="1" customFormat="1" ht="15.75" spans="1:14">
+    <row r="36" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>98</v>
       </c>
@@ -2936,45 +2355,37 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N36">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:N36"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>